<commit_message>
Updated calibration data. Reversed pitch and yaw sign due to quaternion orientation of BNO055 (still figuring this out).
</commit_message>
<xml_diff>
--- a/Project8/bno_cal_data.xlsx
+++ b/Project8/bno_cal_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\School\Johns Hopkins\Computer Science\Software Development for Real Time Systems\RPi\Project8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\School\Johns Hopkins\Computer Science\Software Development for Real Time Systems\Arduino\Project8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895543DE-2D96-4A61-BB2B-08F846DB2D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BEE5AF-A9AD-4F69-86C3-1B8652BE981C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{9D1D1AD7-F77E-4A7F-A473-655231B9999B}"/>
   </bookViews>
@@ -384,12 +384,6 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -406,6 +400,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,354 +720,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30288B58-DF8E-498B-8AF4-5B67463DB12A}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="7">
-        <v>-33</v>
+      <c r="A2" s="19"/>
+      <c r="B2" s="5">
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>-24</v>
-      </c>
-      <c r="D2" s="8">
-        <v>-37</v>
-      </c>
-      <c r="E2" s="7">
-        <v>-4</v>
+        <v>-48</v>
+      </c>
+      <c r="D2" s="6">
+        <v>-42</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-20</v>
       </c>
       <c r="F2" s="1">
         <v>159</v>
       </c>
-      <c r="G2" s="8">
-        <v>-46</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="G2" s="6">
+        <v>-101</v>
+      </c>
+      <c r="H2" s="5">
         <v>-1</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0</v>
-      </c>
-      <c r="K2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
         <v>1000</v>
       </c>
-      <c r="L2" s="10">
-        <v>863</v>
+      <c r="L2" s="8">
+        <v>818</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="7">
-        <v>-39</v>
+      <c r="A3" s="19"/>
+      <c r="B3" s="5">
+        <v>-13</v>
       </c>
       <c r="C3" s="1">
-        <v>-48</v>
-      </c>
-      <c r="D3" s="8">
-        <v>-18</v>
-      </c>
-      <c r="E3" s="7">
-        <v>-4</v>
+        <v>-47</v>
+      </c>
+      <c r="D3" s="6">
+        <v>-14</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-19</v>
       </c>
       <c r="F3" s="1">
-        <v>188</v>
-      </c>
-      <c r="G3" s="8">
-        <v>-91</v>
-      </c>
-      <c r="H3" s="7">
-        <v>-2</v>
+        <v>177</v>
+      </c>
+      <c r="G3" s="6">
+        <v>-114</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
         <v>1000</v>
       </c>
-      <c r="L3" s="10">
-        <v>677</v>
+      <c r="L3" s="8">
+        <v>994</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7">
-        <v>-9</v>
+      <c r="A4" s="19"/>
+      <c r="B4" s="5">
+        <v>-6</v>
       </c>
       <c r="C4" s="1">
-        <v>-25</v>
-      </c>
-      <c r="D4" s="8">
-        <v>-42</v>
-      </c>
-      <c r="E4" s="7">
-        <v>-3</v>
+        <v>-34</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-24</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-15</v>
       </c>
       <c r="F4" s="1">
-        <v>169</v>
-      </c>
-      <c r="G4" s="8">
-        <v>-75</v>
-      </c>
-      <c r="H4" s="7">
-        <v>-1</v>
+        <v>156</v>
+      </c>
+      <c r="G4" s="6">
+        <v>-106</v>
+      </c>
+      <c r="H4" s="5">
+        <v>-2</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
         <v>1000</v>
       </c>
-      <c r="L4" s="10">
-        <v>791</v>
+      <c r="L4" s="8">
+        <v>869</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7">
-        <v>-19</v>
+      <c r="A5" s="19"/>
+      <c r="B5" s="5">
+        <v>-8</v>
       </c>
       <c r="C5" s="1">
-        <v>-32</v>
-      </c>
-      <c r="D5" s="8">
-        <v>-49</v>
-      </c>
-      <c r="E5" s="7">
-        <v>-13</v>
+        <v>-43</v>
+      </c>
+      <c r="D5" s="6">
+        <v>-31</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-34</v>
       </c>
       <c r="F5" s="1">
-        <v>161</v>
-      </c>
-      <c r="G5" s="8">
-        <v>-70</v>
-      </c>
-      <c r="H5" s="7">
-        <v>-2</v>
+        <v>151</v>
+      </c>
+      <c r="G5" s="6">
+        <v>-104</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>-1</v>
       </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10">
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
         <v>1000</v>
       </c>
-      <c r="L5" s="10">
-        <v>823</v>
+      <c r="L5" s="8">
+        <v>805</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7">
+      <c r="A6" s="19"/>
+      <c r="B6" s="5">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-38</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-33</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-37</v>
+      </c>
+      <c r="F6" s="1">
+        <v>156</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-108</v>
+      </c>
+      <c r="H6" s="5">
         <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>-29</v>
-      </c>
-      <c r="E6" s="7">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>162</v>
-      </c>
-      <c r="G6" s="8">
-        <v>-70</v>
-      </c>
-      <c r="H6" s="7">
-        <v>-1</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
         <v>1000</v>
       </c>
-      <c r="L6" s="10">
-        <v>807</v>
+      <c r="L6" s="8">
+        <v>818</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7">
-        <v>-4</v>
+      <c r="A7" s="19"/>
+      <c r="B7" s="5">
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>-64</v>
-      </c>
-      <c r="D7" s="8">
-        <v>-38</v>
-      </c>
-      <c r="E7" s="7">
-        <v>-15</v>
+        <v>-47</v>
+      </c>
+      <c r="D7" s="6">
+        <v>-34</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-33</v>
       </c>
       <c r="F7" s="1">
-        <v>177</v>
-      </c>
-      <c r="G7" s="8">
-        <v>-71</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
+        <v>156</v>
+      </c>
+      <c r="G7" s="6">
+        <v>-103</v>
+      </c>
+      <c r="H7" s="5">
+        <v>-2</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
+        <v>-2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
         <v>1000</v>
       </c>
-      <c r="L7" s="10">
-        <v>819</v>
+      <c r="L7" s="8">
+        <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="9">
+        <v>-11</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-43</v>
+      </c>
+      <c r="D8" s="11">
+        <v>-32</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-31</v>
+      </c>
+      <c r="F8" s="10">
+        <v>155</v>
+      </c>
+      <c r="G8" s="11">
+        <v>-108</v>
+      </c>
+      <c r="H8" s="9">
+        <v>3</v>
+      </c>
+      <c r="I8" s="10">
+        <v>-1</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1000</v>
+      </c>
+      <c r="L8" s="12">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="9">
+        <v>-5</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-37</v>
+      </c>
+      <c r="D9" s="11">
+        <v>-24</v>
+      </c>
+      <c r="E9" s="9">
         <v>-34</v>
       </c>
-      <c r="C8" s="12">
-        <v>-32</v>
-      </c>
-      <c r="D8" s="13">
-        <v>-36</v>
-      </c>
-      <c r="E8" s="11">
-        <v>-41</v>
-      </c>
-      <c r="F8" s="12">
-        <v>183</v>
-      </c>
-      <c r="G8" s="13">
-        <v>-68</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="F9" s="10">
+        <v>163</v>
+      </c>
+      <c r="G9" s="11">
+        <v>-105</v>
+      </c>
+      <c r="H9" s="9">
         <v>-1</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1000</v>
+      </c>
+      <c r="L9" s="12">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="9">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-43</v>
+      </c>
+      <c r="D10" s="11">
+        <v>-14</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-40</v>
+      </c>
+      <c r="F10" s="10">
+        <v>175</v>
+      </c>
+      <c r="G10" s="11">
+        <v>-105</v>
+      </c>
+      <c r="H10" s="9">
+        <v>-2</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1000</v>
+      </c>
+      <c r="L10" s="12">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="9">
+        <v>-7</v>
+      </c>
+      <c r="C11" s="10">
+        <v>-33</v>
+      </c>
+      <c r="D11" s="11">
+        <v>-21</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-21</v>
+      </c>
+      <c r="F11" s="10">
+        <v>172</v>
+      </c>
+      <c r="G11" s="11">
+        <v>-102</v>
+      </c>
+      <c r="H11" s="9">
+        <v>-1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
         <v>1</v>
       </c>
-      <c r="J8" s="13">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="K11" s="12">
         <v>1000</v>
       </c>
-      <c r="L8" s="14">
-        <v>859</v>
+      <c r="L11" s="12">
+        <v>881</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="16">
-        <f>AVERAGE(B2:B8)</f>
-        <v>-19.428571428571427</v>
-      </c>
-      <c r="C9" s="17">
-        <f t="shared" ref="C9:L9" si="0">AVERAGE(C2:C8)</f>
-        <v>-32.714285714285715</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="B12" s="14">
+        <f>AVERAGE(B2:B11)</f>
+        <v>-1.9</v>
+      </c>
+      <c r="C12" s="15">
+        <f t="shared" ref="C12:L12" si="0">AVERAGE(C2:C11)</f>
+        <v>-41.3</v>
+      </c>
+      <c r="D12" s="16">
         <f t="shared" si="0"/>
-        <v>-35.571428571428569</v>
-      </c>
-      <c r="E9" s="16">
+        <v>-26.9</v>
+      </c>
+      <c r="E12" s="14">
         <f t="shared" si="0"/>
-        <v>-10.714285714285714</v>
-      </c>
-      <c r="F9" s="17">
+        <v>-28.4</v>
+      </c>
+      <c r="F12" s="15">
         <f t="shared" si="0"/>
-        <v>171.28571428571428</v>
-      </c>
-      <c r="G9" s="18">
+        <v>162</v>
+      </c>
+      <c r="G12" s="16">
         <f t="shared" si="0"/>
-        <v>-70.142857142857139</v>
-      </c>
-      <c r="H9" s="16">
+        <v>-105.6</v>
+      </c>
+      <c r="H12" s="14">
         <f t="shared" si="0"/>
-        <v>-1.1428571428571428</v>
-      </c>
-      <c r="I9" s="17">
+        <v>-0.2</v>
+      </c>
+      <c r="I12" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="18">
+        <v>-0.2</v>
+      </c>
+      <c r="J12" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="17">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L12" s="17">
         <f t="shared" si="0"/>
-        <v>805.57142857142856</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A8"/>
+    <mergeCell ref="A1:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial commit of project 10.
</commit_message>
<xml_diff>
--- a/Project8/bno_cal_data.xlsx
+++ b/Project8/bno_cal_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\School\Johns Hopkins\Computer Science\Software Development for Real Time Systems\Arduino\Project8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BEE5AF-A9AD-4F69-86C3-1B8652BE981C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14A96D-5C34-4A95-9C5C-3CE221599B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{9D1D1AD7-F77E-4A7F-A473-655231B9999B}"/>
   </bookViews>
@@ -723,7 +723,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>